<commit_message>
fix SUM Export Data Rekap NG
</commit_message>
<xml_diff>
--- a/storage/template/Export_Rekap_NG_CSH_D98E.xlsx
+++ b/storage/template/Export_Rekap_NG_CSH_D98E.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\02_Sotfware\laravel\avicenna\storage\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D06AA46C-A91D-4EEC-9F13-08473B196EF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E7AE819-AE5F-4CFA-971A-4F3C100AC7E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{05F26BD9-E112-4214-87F4-B2A2D3F2905B}"/>
   </bookViews>
@@ -208,7 +208,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="39">
+  <borders count="38">
     <border>
       <left/>
       <right/>
@@ -676,17 +676,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -720,7 +709,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -794,15 +783,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -863,9 +843,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -881,31 +858,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill>
@@ -1333,16 +1305,16 @@
   <sheetData>
     <row r="17" spans="1:38" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="18" spans="1:38" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="25" t="s">
+      <c r="A18" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="26"/>
-      <c r="C18" s="26"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="26"/>
-      <c r="H18" s="27"/>
+      <c r="B18" s="51"/>
+      <c r="C18" s="51"/>
+      <c r="D18" s="51"/>
+      <c r="E18" s="51"/>
+      <c r="F18" s="51"/>
+      <c r="G18" s="51"/>
+      <c r="H18" s="52"/>
     </row>
     <row r="19" spans="1:38" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="20" spans="1:38" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1454,7 +1426,7 @@
       <c r="AK20" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="AL20" s="43" t="s">
+      <c r="AL20" s="40" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1470,10 +1442,10 @@
       <c r="J21" s="16">
         <v>6</v>
       </c>
-      <c r="K21" s="34">
+      <c r="K21" s="31">
         <v>14</v>
       </c>
-      <c r="L21" s="49">
+      <c r="L21" s="45">
         <f>COUNTIFS($C$21:$C$500,$J21,$E$21:$E$500,$K21,$H$21:$H$500,L$20)</f>
         <v>0</v>
       </c>
@@ -1538,19 +1510,19 @@
         <v>0</v>
       </c>
       <c r="AB21" s="19">
-        <f>COUNTIFS($C$21:$C$500,$J21,$E$21:$E$500,$K21,$H$21:$H$500,"*" &amp; AB$20 &amp; "*")</f>
+        <f t="shared" ref="AB21:AE47" si="1">COUNTIFS($C$21:$C$500,$J21,$E$21:$E$500,$K21,$H$21:$H$500,"*" &amp; AB$20 &amp; "*")</f>
         <v>0</v>
       </c>
       <c r="AC21" s="19">
-        <f>COUNTIFS($C$21:$C$500,$J21,$E$21:$E$500,$K21,$H$21:$H$500,"*" &amp; AC$20 &amp; "*")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AD21" s="19">
-        <f>COUNTIFS($C$21:$C$500,$J21,$E$21:$E$500,$K21,$H$21:$H$500,"*" &amp; AD$20 &amp; "*")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AE21" s="19">
-        <f>COUNTIFS($C$21:$C$500,$J21,$E$21:$E$500,$K21,$H$21:$H$500,"*" &amp; AE$20 &amp; "*")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AF21" s="19">
@@ -1558,27 +1530,27 @@
         <v>0</v>
       </c>
       <c r="AG21" s="19">
-        <f t="shared" ref="AG21:AK36" si="1">COUNTIFS($C$21:$C$500,$J21,$E$21:$E$500,$K21,$H$21:$H$500,AG$20)</f>
+        <f t="shared" ref="AG21:AK36" si="2">COUNTIFS($C$21:$C$500,$J21,$E$21:$E$500,$K21,$H$21:$H$500,AG$20)</f>
         <v>0</v>
       </c>
       <c r="AH21" s="19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AI21" s="19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AJ21" s="19">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AK21" s="31">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AL21" s="44">
-        <f>SUM(L21:AF21)</f>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AK21" s="28">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AL21" s="41">
+        <f>SUM(L21:AK21)</f>
         <v>0</v>
       </c>
     </row>
@@ -1594,43 +1566,43 @@
       <c r="J22" s="5">
         <v>6</v>
       </c>
-      <c r="K22" s="35">
+      <c r="K22" s="32">
         <v>15</v>
       </c>
-      <c r="L22" s="50">
-        <f t="shared" ref="L22:W47" si="2">COUNTIFS($C$21:$C$500,$J22,$E$21:$E$500,$K22,$H$21:$H$500,L$20)</f>
+      <c r="L22" s="46">
+        <f t="shared" ref="L22:T47" si="3">COUNTIFS($C$21:$C$500,$J22,$E$21:$E$500,$K22,$H$21:$H$500,L$20)</f>
         <v>0</v>
       </c>
       <c r="M22" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N22" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="O22" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="P22" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Q22" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R22" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="S22" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="T22" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="U22" s="3">
@@ -1662,47 +1634,47 @@
         <v>0</v>
       </c>
       <c r="AB22" s="3">
-        <f>COUNTIFS($C$21:$C$500,$J22,$E$21:$E$500,$K22,$H$21:$H$500,"*" &amp; AB$20 &amp; "*")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AC22" s="3">
-        <f>COUNTIFS($C$21:$C$500,$J22,$E$21:$E$500,$K22,$H$21:$H$500,"*" &amp; AC$20 &amp; "*")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AD22" s="3">
-        <f>COUNTIFS($C$21:$C$500,$J22,$E$21:$E$500,$K22,$H$21:$H$500,"*" &amp; AD$20 &amp; "*")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AE22" s="3">
-        <f>COUNTIFS($C$21:$C$500,$J22,$E$21:$E$500,$K22,$H$21:$H$500,"*" &amp; AE$20 &amp; "*")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AF22" s="3">
-        <f t="shared" ref="AF22:AK47" si="3">COUNTIFS($C$21:$C$500,$J22,$E$21:$E$500,$K22,$H$21:$H$500,AF$20)</f>
+        <f t="shared" ref="AF22:AK47" si="4">COUNTIFS($C$21:$C$500,$J22,$E$21:$E$500,$K22,$H$21:$H$500,AF$20)</f>
         <v>0</v>
       </c>
       <c r="AG22" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AH22" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AI22" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AJ22" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AK22" s="28">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AL22" s="45">
-        <f>SUM(L22:AE22)</f>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AK22" s="25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AL22" s="42">
+        <f>SUM(L22:AK22)</f>
         <v>0</v>
       </c>
     </row>
@@ -1718,39 +1690,39 @@
       <c r="J23" s="5">
         <v>6</v>
       </c>
-      <c r="K23" s="35">
+      <c r="K23" s="32">
         <v>16</v>
       </c>
-      <c r="L23" s="50">
-        <f t="shared" si="2"/>
+      <c r="L23" s="46">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M23" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N23" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="O23" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="P23" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Q23" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R23" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="S23" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="T23" s="3">
@@ -1786,47 +1758,47 @@
         <v>0</v>
       </c>
       <c r="AB23" s="3">
-        <f>COUNTIFS($C$21:$C$500,$J23,$E$21:$E$500,$K23,$H$21:$H$500,"*" &amp; AB$20 &amp; "*")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AC23" s="3">
-        <f>COUNTIFS($C$21:$C$500,$J23,$E$21:$E$500,$K23,$H$21:$H$500,"*" &amp; AC$20 &amp; "*")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AD23" s="3">
-        <f>COUNTIFS($C$21:$C$500,$J23,$E$21:$E$500,$K23,$H$21:$H$500,"*" &amp; AD$20 &amp; "*")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AE23" s="3">
-        <f>COUNTIFS($C$21:$C$500,$J23,$E$21:$E$500,$K23,$H$21:$H$500,"*" &amp; AE$20 &amp; "*")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AF23" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AG23" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AH23" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AI23" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AJ23" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AK23" s="28">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AL23" s="45">
-        <f>SUM(L23:AE23)</f>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AK23" s="25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AL23" s="42">
+        <f t="shared" ref="AL23:AL27" si="5">SUM(L23:AK23)</f>
         <v>0</v>
       </c>
     </row>
@@ -1842,39 +1814,39 @@
       <c r="J24" s="5">
         <v>6</v>
       </c>
-      <c r="K24" s="35">
+      <c r="K24" s="32">
         <v>17</v>
       </c>
-      <c r="L24" s="50">
-        <f t="shared" si="2"/>
+      <c r="L24" s="46">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M24" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N24" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="O24" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="P24" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Q24" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R24" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="S24" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="T24" s="3">
@@ -1910,47 +1882,47 @@
         <v>0</v>
       </c>
       <c r="AB24" s="3">
-        <f>COUNTIFS($C$21:$C$500,$J24,$E$21:$E$500,$K24,$H$21:$H$500,"*" &amp; AB$20 &amp; "*")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AC24" s="3">
-        <f>COUNTIFS($C$21:$C$500,$J24,$E$21:$E$500,$K24,$H$21:$H$500,"*" &amp; AC$20 &amp; "*")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AD24" s="3">
-        <f>COUNTIFS($C$21:$C$500,$J24,$E$21:$E$500,$K24,$H$21:$H$500,"*" &amp; AD$20 &amp; "*")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AE24" s="3">
-        <f>COUNTIFS($C$21:$C$500,$J24,$E$21:$E$500,$K24,$H$21:$H$500,"*" &amp; AE$20 &amp; "*")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AF24" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AG24" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AH24" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AI24" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AJ24" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AK24" s="28">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AL24" s="45">
-        <f>SUM(L24:AE24)</f>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AK24" s="25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AL24" s="42">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -1966,39 +1938,39 @@
       <c r="J25" s="5">
         <v>6</v>
       </c>
-      <c r="K25" s="35">
+      <c r="K25" s="32">
         <v>18</v>
       </c>
-      <c r="L25" s="50">
-        <f t="shared" si="2"/>
+      <c r="L25" s="46">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M25" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N25" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="O25" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="P25" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Q25" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R25" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="S25" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="T25" s="3">
@@ -2034,47 +2006,47 @@
         <v>0</v>
       </c>
       <c r="AB25" s="3">
-        <f>COUNTIFS($C$21:$C$500,$J25,$E$21:$E$500,$K25,$H$21:$H$500,"*" &amp; AB$20 &amp; "*")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AC25" s="3">
-        <f>COUNTIFS($C$21:$C$500,$J25,$E$21:$E$500,$K25,$H$21:$H$500,"*" &amp; AC$20 &amp; "*")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AD25" s="3">
-        <f>COUNTIFS($C$21:$C$500,$J25,$E$21:$E$500,$K25,$H$21:$H$500,"*" &amp; AD$20 &amp; "*")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AE25" s="3">
-        <f>COUNTIFS($C$21:$C$500,$J25,$E$21:$E$500,$K25,$H$21:$H$500,"*" &amp; AE$20 &amp; "*")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AF25" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AG25" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AH25" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AI25" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AJ25" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AK25" s="28">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AL25" s="45">
-        <f>SUM(L25:AE25)</f>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AK25" s="25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AL25" s="42">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -2090,39 +2062,39 @@
       <c r="J26" s="5">
         <v>6</v>
       </c>
-      <c r="K26" s="35">
+      <c r="K26" s="32">
         <v>19</v>
       </c>
-      <c r="L26" s="50">
-        <f t="shared" si="2"/>
+      <c r="L26" s="46">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M26" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N26" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="O26" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="P26" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Q26" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R26" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="S26" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="T26" s="3">
@@ -2158,47 +2130,47 @@
         <v>0</v>
       </c>
       <c r="AB26" s="3">
-        <f>COUNTIFS($C$21:$C$500,$J26,$E$21:$E$500,$K26,$H$21:$H$500,"*" &amp; AB$20 &amp; "*")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AC26" s="3">
-        <f>COUNTIFS($C$21:$C$500,$J26,$E$21:$E$500,$K26,$H$21:$H$500,"*" &amp; AC$20 &amp; "*")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AD26" s="3">
-        <f>COUNTIFS($C$21:$C$500,$J26,$E$21:$E$500,$K26,$H$21:$H$500,"*" &amp; AD$20 &amp; "*")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AE26" s="3">
-        <f>COUNTIFS($C$21:$C$500,$J26,$E$21:$E$500,$K26,$H$21:$H$500,"*" &amp; AE$20 &amp; "*")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AF26" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AG26" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AH26" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AI26" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AJ26" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AK26" s="28">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AL26" s="45">
-        <f>SUM(L26:AE26)</f>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AK26" s="25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AL26" s="42">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -2214,39 +2186,39 @@
       <c r="J27" s="5">
         <v>6</v>
       </c>
-      <c r="K27" s="35">
+      <c r="K27" s="32">
         <v>20</v>
       </c>
-      <c r="L27" s="50">
-        <f t="shared" si="2"/>
+      <c r="L27" s="46">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M27" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N27" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="O27" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="P27" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Q27" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R27" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="S27" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="T27" s="3">
@@ -2282,47 +2254,47 @@
         <v>0</v>
       </c>
       <c r="AB27" s="3">
-        <f>COUNTIFS($C$21:$C$500,$J27,$E$21:$E$500,$K27,$H$21:$H$500,"*" &amp; AB$20 &amp; "*")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AC27" s="3">
-        <f>COUNTIFS($C$21:$C$500,$J27,$E$21:$E$500,$K27,$H$21:$H$500,"*" &amp; AC$20 &amp; "*")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AD27" s="3">
-        <f>COUNTIFS($C$21:$C$500,$J27,$E$21:$E$500,$K27,$H$21:$H$500,"*" &amp; AD$20 &amp; "*")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AE27" s="3">
-        <f>COUNTIFS($C$21:$C$500,$J27,$E$21:$E$500,$K27,$H$21:$H$500,"*" &amp; AE$20 &amp; "*")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AF27" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AG27" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AH27" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AI27" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AJ27" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AK27" s="28">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AL27" s="45">
-        <f>SUM(L27:AE27)</f>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AK27" s="25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AL27" s="42">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -2338,39 +2310,39 @@
       <c r="J28" s="5">
         <v>6</v>
       </c>
-      <c r="K28" s="35">
+      <c r="K28" s="32">
         <v>21</v>
       </c>
-      <c r="L28" s="50">
-        <f t="shared" si="2"/>
+      <c r="L28" s="46">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M28" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N28" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="O28" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="P28" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Q28" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R28" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="S28" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="T28" s="3">
@@ -2406,47 +2378,47 @@
         <v>0</v>
       </c>
       <c r="AB28" s="3">
-        <f>COUNTIFS($C$21:$C$500,$J28,$E$21:$E$500,$K28,$H$21:$H$500,"*" &amp; AB$20 &amp; "*")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AC28" s="3">
-        <f>COUNTIFS($C$21:$C$500,$J28,$E$21:$E$500,$K28,$H$21:$H$500,"*" &amp; AC$20 &amp; "*")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AD28" s="3">
-        <f>COUNTIFS($C$21:$C$500,$J28,$E$21:$E$500,$K28,$H$21:$H$500,"*" &amp; AD$20 &amp; "*")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AE28" s="3">
-        <f>COUNTIFS($C$21:$C$500,$J28,$E$21:$E$500,$K28,$H$21:$H$500,"*" &amp; AE$20 &amp; "*")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AF28" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AG28" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AH28" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AI28" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AJ28" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AK28" s="28">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AL28" s="45">
-        <f>SUM(L28:AE28)</f>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AK28" s="25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AL28" s="42">
+        <f>SUM(L28:AK28)</f>
         <v>0</v>
       </c>
     </row>
@@ -2462,39 +2434,39 @@
       <c r="J29" s="6">
         <v>6</v>
       </c>
-      <c r="K29" s="36">
+      <c r="K29" s="33">
         <v>22</v>
       </c>
-      <c r="L29" s="51">
-        <f t="shared" si="2"/>
+      <c r="L29" s="47">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M29" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N29" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="O29" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="P29" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Q29" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R29" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="S29" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="T29" s="20">
@@ -2530,47 +2502,47 @@
         <v>0</v>
       </c>
       <c r="AB29" s="20">
-        <f>COUNTIFS($C$21:$C$500,$J29,$E$21:$E$500,$K29,$H$21:$H$500,"*" &amp; AB$20 &amp; "*")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AC29" s="20">
-        <f>COUNTIFS($C$21:$C$500,$J29,$E$21:$E$500,$K29,$H$21:$H$500,"*" &amp; AC$20 &amp; "*")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AD29" s="20">
-        <f>COUNTIFS($C$21:$C$500,$J29,$E$21:$E$500,$K29,$H$21:$H$500,"*" &amp; AD$20 &amp; "*")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AE29" s="20">
-        <f>COUNTIFS($C$21:$C$500,$J29,$E$21:$E$500,$K29,$H$21:$H$500,"*" &amp; AE$20 &amp; "*")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AF29" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AG29" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AH29" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AI29" s="20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AJ29" s="20">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AK29" s="29">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AL29" s="46">
-        <f>SUM(L29:AE29)</f>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AK29" s="26">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AL29" s="43">
+        <f>SUM(L29:AK29)</f>
         <v>0</v>
       </c>
     </row>
@@ -2586,39 +2558,39 @@
       <c r="J30" s="15">
         <v>7</v>
       </c>
-      <c r="K30" s="37">
+      <c r="K30" s="34">
         <v>14</v>
       </c>
-      <c r="L30" s="52">
-        <f t="shared" si="2"/>
+      <c r="L30" s="48">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M30" s="21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N30" s="21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="O30" s="21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="P30" s="21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Q30" s="21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R30" s="21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="S30" s="21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="T30" s="21">
@@ -2654,47 +2626,47 @@
         <v>0</v>
       </c>
       <c r="AB30" s="21">
-        <f>COUNTIFS($C$21:$C$500,$J30,$E$21:$E$500,$K30,$H$21:$H$500,"*" &amp; AB$20 &amp; "*")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AC30" s="21">
-        <f>COUNTIFS($C$21:$C$500,$J30,$E$21:$E$500,$K30,$H$21:$H$500,"*" &amp; AC$20 &amp; "*")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AD30" s="21">
-        <f>COUNTIFS($C$21:$C$500,$J30,$E$21:$E$500,$K30,$H$21:$H$500,"*" &amp; AD$20 &amp; "*")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AE30" s="21">
-        <f>COUNTIFS($C$21:$C$500,$J30,$E$21:$E$500,$K30,$H$21:$H$500,"*" &amp; AE$20 &amp; "*")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AF30" s="21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AG30" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AH30" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AI30" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AJ30" s="21">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AK30" s="30">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AL30" s="47">
-        <f>SUM(L30:AE30)</f>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AK30" s="27">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AL30" s="44">
+        <f>SUM(L30:AK30)</f>
         <v>0</v>
       </c>
     </row>
@@ -2710,39 +2682,39 @@
       <c r="J31" s="7">
         <v>7</v>
       </c>
-      <c r="K31" s="38">
+      <c r="K31" s="35">
         <v>15</v>
       </c>
-      <c r="L31" s="50">
-        <f t="shared" si="2"/>
+      <c r="L31" s="46">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M31" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N31" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="O31" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="P31" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Q31" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R31" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="S31" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="T31" s="3">
@@ -2778,47 +2750,47 @@
         <v>0</v>
       </c>
       <c r="AB31" s="3">
-        <f>COUNTIFS($C$21:$C$500,$J31,$E$21:$E$500,$K31,$H$21:$H$500,"*" &amp; AB$20 &amp; "*")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AC31" s="3">
-        <f>COUNTIFS($C$21:$C$500,$J31,$E$21:$E$500,$K31,$H$21:$H$500,"*" &amp; AC$20 &amp; "*")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AD31" s="3">
-        <f>COUNTIFS($C$21:$C$500,$J31,$E$21:$E$500,$K31,$H$21:$H$500,"*" &amp; AD$20 &amp; "*")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AE31" s="3">
-        <f>COUNTIFS($C$21:$C$500,$J31,$E$21:$E$500,$K31,$H$21:$H$500,"*" &amp; AE$20 &amp; "*")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AF31" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AG31" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AH31" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AI31" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AJ31" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AK31" s="28">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AL31" s="45">
-        <f>SUM(L31:AE31)</f>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AK31" s="25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AL31" s="42">
+        <f>SUM(L31:AK31)</f>
         <v>0</v>
       </c>
     </row>
@@ -2834,39 +2806,39 @@
       <c r="J32" s="7">
         <v>7</v>
       </c>
-      <c r="K32" s="38">
+      <c r="K32" s="35">
         <v>16</v>
       </c>
-      <c r="L32" s="50">
-        <f t="shared" si="2"/>
+      <c r="L32" s="46">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M32" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N32" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="O32" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="P32" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Q32" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R32" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="S32" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="T32" s="3">
@@ -2902,47 +2874,47 @@
         <v>0</v>
       </c>
       <c r="AB32" s="3">
-        <f>COUNTIFS($C$21:$C$500,$J32,$E$21:$E$500,$K32,$H$21:$H$500,"*" &amp; AB$20 &amp; "*")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AC32" s="3">
-        <f>COUNTIFS($C$21:$C$500,$J32,$E$21:$E$500,$K32,$H$21:$H$500,"*" &amp; AC$20 &amp; "*")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AD32" s="3">
-        <f>COUNTIFS($C$21:$C$500,$J32,$E$21:$E$500,$K32,$H$21:$H$500,"*" &amp; AD$20 &amp; "*")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AE32" s="3">
-        <f>COUNTIFS($C$21:$C$500,$J32,$E$21:$E$500,$K32,$H$21:$H$500,"*" &amp; AE$20 &amp; "*")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AF32" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AG32" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AH32" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AI32" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AJ32" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AK32" s="28">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AL32" s="45">
-        <f>SUM(L32:AE32)</f>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AK32" s="25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AL32" s="42">
+        <f t="shared" ref="AL32:AL37" si="6">SUM(L32:AK32)</f>
         <v>0</v>
       </c>
     </row>
@@ -2958,39 +2930,39 @@
       <c r="J33" s="7">
         <v>7</v>
       </c>
-      <c r="K33" s="38">
+      <c r="K33" s="35">
         <v>17</v>
       </c>
-      <c r="L33" s="50">
-        <f t="shared" si="2"/>
+      <c r="L33" s="46">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M33" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N33" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="O33" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="P33" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Q33" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R33" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="S33" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="T33" s="3">
@@ -3026,47 +2998,47 @@
         <v>0</v>
       </c>
       <c r="AB33" s="3">
-        <f>COUNTIFS($C$21:$C$500,$J33,$E$21:$E$500,$K33,$H$21:$H$500,"*" &amp; AB$20 &amp; "*")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AC33" s="3">
-        <f>COUNTIFS($C$21:$C$500,$J33,$E$21:$E$500,$K33,$H$21:$H$500,"*" &amp; AC$20 &amp; "*")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AD33" s="3">
-        <f>COUNTIFS($C$21:$C$500,$J33,$E$21:$E$500,$K33,$H$21:$H$500,"*" &amp; AD$20 &amp; "*")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AE33" s="3">
-        <f>COUNTIFS($C$21:$C$500,$J33,$E$21:$E$500,$K33,$H$21:$H$500,"*" &amp; AE$20 &amp; "*")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AF33" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AG33" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AH33" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AI33" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AJ33" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AK33" s="28">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AL33" s="45">
-        <f>SUM(L33:AE33)</f>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AK33" s="25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AL33" s="42">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -3082,39 +3054,39 @@
       <c r="J34" s="7">
         <v>7</v>
       </c>
-      <c r="K34" s="38">
+      <c r="K34" s="35">
         <v>18</v>
       </c>
-      <c r="L34" s="50">
-        <f t="shared" si="2"/>
+      <c r="L34" s="46">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M34" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N34" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="O34" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="P34" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Q34" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R34" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="S34" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="T34" s="3">
@@ -3150,47 +3122,47 @@
         <v>0</v>
       </c>
       <c r="AB34" s="3">
-        <f>COUNTIFS($C$21:$C$500,$J34,$E$21:$E$500,$K34,$H$21:$H$500,"*" &amp; AB$20 &amp; "*")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AC34" s="3">
-        <f>COUNTIFS($C$21:$C$500,$J34,$E$21:$E$500,$K34,$H$21:$H$500,"*" &amp; AC$20 &amp; "*")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AD34" s="3">
-        <f>COUNTIFS($C$21:$C$500,$J34,$E$21:$E$500,$K34,$H$21:$H$500,"*" &amp; AD$20 &amp; "*")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AE34" s="3">
-        <f>COUNTIFS($C$21:$C$500,$J34,$E$21:$E$500,$K34,$H$21:$H$500,"*" &amp; AE$20 &amp; "*")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AF34" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AG34" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AH34" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AI34" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AJ34" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AK34" s="28">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AL34" s="45">
-        <f>SUM(L34:AE34)</f>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AK34" s="25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AL34" s="42">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -3206,39 +3178,39 @@
       <c r="J35" s="7">
         <v>7</v>
       </c>
-      <c r="K35" s="38">
+      <c r="K35" s="35">
         <v>19</v>
       </c>
-      <c r="L35" s="50">
-        <f t="shared" si="2"/>
+      <c r="L35" s="46">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M35" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N35" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="O35" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="P35" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Q35" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R35" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="S35" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="T35" s="3">
@@ -3274,47 +3246,47 @@
         <v>0</v>
       </c>
       <c r="AB35" s="3">
-        <f>COUNTIFS($C$21:$C$500,$J35,$E$21:$E$500,$K35,$H$21:$H$500,"*" &amp; AB$20 &amp; "*")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AC35" s="3">
-        <f>COUNTIFS($C$21:$C$500,$J35,$E$21:$E$500,$K35,$H$21:$H$500,"*" &amp; AC$20 &amp; "*")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AD35" s="3">
-        <f>COUNTIFS($C$21:$C$500,$J35,$E$21:$E$500,$K35,$H$21:$H$500,"*" &amp; AD$20 &amp; "*")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AE35" s="3">
-        <f>COUNTIFS($C$21:$C$500,$J35,$E$21:$E$500,$K35,$H$21:$H$500,"*" &amp; AE$20 &amp; "*")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AF35" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AG35" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AH35" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AI35" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AJ35" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AK35" s="28">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AL35" s="45">
-        <f>SUM(L35:AE35)</f>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AK35" s="25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AL35" s="42">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -3330,39 +3302,39 @@
       <c r="J36" s="7">
         <v>7</v>
       </c>
-      <c r="K36" s="38">
+      <c r="K36" s="35">
         <v>20</v>
       </c>
-      <c r="L36" s="50">
-        <f t="shared" si="2"/>
+      <c r="L36" s="46">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M36" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N36" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="O36" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="P36" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Q36" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R36" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="S36" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="T36" s="3">
@@ -3398,47 +3370,47 @@
         <v>0</v>
       </c>
       <c r="AB36" s="3">
-        <f>COUNTIFS($C$21:$C$500,$J36,$E$21:$E$500,$K36,$H$21:$H$500,"*" &amp; AB$20 &amp; "*")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AC36" s="3">
-        <f>COUNTIFS($C$21:$C$500,$J36,$E$21:$E$500,$K36,$H$21:$H$500,"*" &amp; AC$20 &amp; "*")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AD36" s="3">
-        <f>COUNTIFS($C$21:$C$500,$J36,$E$21:$E$500,$K36,$H$21:$H$500,"*" &amp; AD$20 &amp; "*")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AE36" s="3">
-        <f>COUNTIFS($C$21:$C$500,$J36,$E$21:$E$500,$K36,$H$21:$H$500,"*" &amp; AE$20 &amp; "*")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AF36" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AG36" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AH36" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AI36" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AJ36" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AK36" s="28">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AL36" s="45">
-        <f>SUM(L36:AE36)</f>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AK36" s="25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AL36" s="42">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -3454,115 +3426,115 @@
       <c r="J37" s="7">
         <v>7</v>
       </c>
-      <c r="K37" s="38">
+      <c r="K37" s="35">
         <v>21</v>
       </c>
-      <c r="L37" s="50">
-        <f t="shared" si="2"/>
+      <c r="L37" s="46">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M37" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N37" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="O37" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="P37" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Q37" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R37" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="S37" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="T37" s="3">
-        <f t="shared" ref="T37:AA42" si="4">COUNTIFS($C$21:$C$500,$J37,$E$21:$E$500,$K37,$H$21:$H$500,T$20)</f>
+        <f t="shared" ref="T37:AA42" si="7">COUNTIFS($C$21:$C$500,$J37,$E$21:$E$500,$K37,$H$21:$H$500,T$20)</f>
         <v>0</v>
       </c>
       <c r="U37" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="V37" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="W37" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="X37" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="Y37" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="Z37" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AA37" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AB37" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AC37" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AD37" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AE37" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AF37" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="V37" s="3">
+      <c r="AG37" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="W37" s="3">
+      <c r="AH37" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="X37" s="3">
+      <c r="AI37" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="Y37" s="3">
+      <c r="AJ37" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="Z37" s="3">
+      <c r="AK37" s="25">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="AA37" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AB37" s="3">
-        <f>COUNTIFS($C$21:$C$500,$J37,$E$21:$E$500,$K37,$H$21:$H$500,"*" &amp; AB$20 &amp; "*")</f>
-        <v>0</v>
-      </c>
-      <c r="AC37" s="3">
-        <f>COUNTIFS($C$21:$C$500,$J37,$E$21:$E$500,$K37,$H$21:$H$500,"*" &amp; AC$20 &amp; "*")</f>
-        <v>0</v>
-      </c>
-      <c r="AD37" s="3">
-        <f>COUNTIFS($C$21:$C$500,$J37,$E$21:$E$500,$K37,$H$21:$H$500,"*" &amp; AD$20 &amp; "*")</f>
-        <v>0</v>
-      </c>
-      <c r="AE37" s="3">
-        <f>COUNTIFS($C$21:$C$500,$J37,$E$21:$E$500,$K37,$H$21:$H$500,"*" &amp; AE$20 &amp; "*")</f>
-        <v>0</v>
-      </c>
-      <c r="AF37" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AG37" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AH37" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AI37" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AJ37" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AK37" s="28">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AL37" s="45">
-        <f>SUM(L37:AE37)</f>
+      <c r="AL37" s="42">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -3578,115 +3550,115 @@
       <c r="J38" s="17">
         <v>7</v>
       </c>
-      <c r="K38" s="39">
+      <c r="K38" s="36">
         <v>22</v>
       </c>
-      <c r="L38" s="53">
-        <f t="shared" si="2"/>
+      <c r="L38" s="49">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M38" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N38" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="O38" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="P38" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Q38" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R38" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="S38" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="T38" s="22">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="U38" s="22">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="V38" s="22">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="W38" s="22">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="X38" s="22">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="Y38" s="22">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="Z38" s="22">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AA38" s="22">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AB38" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AC38" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AD38" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AE38" s="22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AF38" s="22">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="U38" s="22">
+      <c r="AG38" s="22">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="V38" s="22">
+      <c r="AH38" s="22">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="W38" s="22">
+      <c r="AI38" s="22">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="X38" s="22">
+      <c r="AJ38" s="22">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="Y38" s="22">
+      <c r="AK38" s="29">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="Z38" s="22">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AA38" s="22">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AB38" s="22">
-        <f>COUNTIFS($C$21:$C$500,$J38,$E$21:$E$500,$K38,$H$21:$H$500,"*" &amp; AB$20 &amp; "*")</f>
-        <v>0</v>
-      </c>
-      <c r="AC38" s="22">
-        <f>COUNTIFS($C$21:$C$500,$J38,$E$21:$E$500,$K38,$H$21:$H$500,"*" &amp; AC$20 &amp; "*")</f>
-        <v>0</v>
-      </c>
-      <c r="AD38" s="22">
-        <f>COUNTIFS($C$21:$C$500,$J38,$E$21:$E$500,$K38,$H$21:$H$500,"*" &amp; AD$20 &amp; "*")</f>
-        <v>0</v>
-      </c>
-      <c r="AE38" s="22">
-        <f>COUNTIFS($C$21:$C$500,$J38,$E$21:$E$500,$K38,$H$21:$H$500,"*" &amp; AE$20 &amp; "*")</f>
-        <v>0</v>
-      </c>
-      <c r="AF38" s="22">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AG38" s="22">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AH38" s="22">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AI38" s="22">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AJ38" s="22">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AK38" s="32">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AL38" s="48">
-        <f>SUM(L38:AE38)</f>
+      <c r="AL38" s="42">
+        <f>SUM(L38:AK38)</f>
         <v>0</v>
       </c>
     </row>
@@ -3702,115 +3674,115 @@
       <c r="J39" s="8">
         <v>8</v>
       </c>
-      <c r="K39" s="40">
+      <c r="K39" s="37">
         <v>14</v>
       </c>
-      <c r="L39" s="49">
-        <f t="shared" si="2"/>
+      <c r="L39" s="45">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M39" s="19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N39" s="19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="O39" s="19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="P39" s="19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Q39" s="19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R39" s="19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="S39" s="19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="T39" s="19">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="U39" s="19">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="V39" s="19">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="W39" s="19">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="X39" s="19">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="Y39" s="19">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="Z39" s="19">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AA39" s="19">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AB39" s="19">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AC39" s="19">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AD39" s="19">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AE39" s="19">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AF39" s="19">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="U39" s="19">
+      <c r="AG39" s="19">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="V39" s="19">
+      <c r="AH39" s="19">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="W39" s="19">
+      <c r="AI39" s="19">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="X39" s="19">
+      <c r="AJ39" s="19">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="Y39" s="19">
+      <c r="AK39" s="28">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="Z39" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AA39" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AB39" s="19">
-        <f>COUNTIFS($C$21:$C$500,$J39,$E$21:$E$500,$K39,$H$21:$H$500,"*" &amp; AB$20 &amp; "*")</f>
-        <v>0</v>
-      </c>
-      <c r="AC39" s="19">
-        <f>COUNTIFS($C$21:$C$500,$J39,$E$21:$E$500,$K39,$H$21:$H$500,"*" &amp; AC$20 &amp; "*")</f>
-        <v>0</v>
-      </c>
-      <c r="AD39" s="19">
-        <f>COUNTIFS($C$21:$C$500,$J39,$E$21:$E$500,$K39,$H$21:$H$500,"*" &amp; AD$20 &amp; "*")</f>
-        <v>0</v>
-      </c>
-      <c r="AE39" s="19">
-        <f>COUNTIFS($C$21:$C$500,$J39,$E$21:$E$500,$K39,$H$21:$H$500,"*" &amp; AE$20 &amp; "*")</f>
-        <v>0</v>
-      </c>
-      <c r="AF39" s="19">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AG39" s="19">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AH39" s="19">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AI39" s="19">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AJ39" s="19">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AK39" s="31">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AL39" s="44">
-        <f>SUM(L39:AE39)</f>
+      <c r="AL39" s="41">
+        <f>SUM(L39:AK39)</f>
         <v>0</v>
       </c>
     </row>
@@ -3826,115 +3798,115 @@
       <c r="J40" s="9">
         <v>8</v>
       </c>
-      <c r="K40" s="41">
+      <c r="K40" s="38">
         <v>15</v>
       </c>
-      <c r="L40" s="50">
-        <f t="shared" si="2"/>
+      <c r="L40" s="46">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M40" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N40" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="O40" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="P40" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Q40" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R40" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="S40" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="T40" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="U40" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="V40" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="W40" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="X40" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="Y40" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="Z40" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AA40" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AB40" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AC40" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AD40" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AE40" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AF40" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="U40" s="3">
+      <c r="AG40" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="V40" s="3">
+      <c r="AH40" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="W40" s="3">
+      <c r="AI40" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="X40" s="3">
+      <c r="AJ40" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="Y40" s="3">
+      <c r="AK40" s="25">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="Z40" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AA40" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AB40" s="3">
-        <f>COUNTIFS($C$21:$C$500,$J40,$E$21:$E$500,$K40,$H$21:$H$500,"*" &amp; AB$20 &amp; "*")</f>
-        <v>0</v>
-      </c>
-      <c r="AC40" s="3">
-        <f>COUNTIFS($C$21:$C$500,$J40,$E$21:$E$500,$K40,$H$21:$H$500,"*" &amp; AC$20 &amp; "*")</f>
-        <v>0</v>
-      </c>
-      <c r="AD40" s="3">
-        <f>COUNTIFS($C$21:$C$500,$J40,$E$21:$E$500,$K40,$H$21:$H$500,"*" &amp; AD$20 &amp; "*")</f>
-        <v>0</v>
-      </c>
-      <c r="AE40" s="3">
-        <f>COUNTIFS($C$21:$C$500,$J40,$E$21:$E$500,$K40,$H$21:$H$500,"*" &amp; AE$20 &amp; "*")</f>
-        <v>0</v>
-      </c>
-      <c r="AF40" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AG40" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AH40" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AI40" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AJ40" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AK40" s="28">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AL40" s="45">
-        <f>SUM(L40:AE40)</f>
+      <c r="AL40" s="42">
+        <f>SUM(L40:AK40)</f>
         <v>0</v>
       </c>
     </row>
@@ -3950,115 +3922,115 @@
       <c r="J41" s="9">
         <v>8</v>
       </c>
-      <c r="K41" s="41">
+      <c r="K41" s="38">
         <v>16</v>
       </c>
-      <c r="L41" s="50">
-        <f t="shared" si="2"/>
+      <c r="L41" s="46">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M41" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N41" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="O41" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="P41" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Q41" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R41" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="S41" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="T41" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="U41" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="V41" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="W41" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="X41" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="Y41" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="Z41" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AA41" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AB41" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AC41" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AD41" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AE41" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AF41" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="U41" s="3">
+      <c r="AG41" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="V41" s="3">
+      <c r="AH41" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="W41" s="3">
+      <c r="AI41" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="X41" s="3">
+      <c r="AJ41" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="Y41" s="3">
+      <c r="AK41" s="25">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="Z41" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AA41" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AB41" s="3">
-        <f>COUNTIFS($C$21:$C$500,$J41,$E$21:$E$500,$K41,$H$21:$H$500,"*" &amp; AB$20 &amp; "*")</f>
-        <v>0</v>
-      </c>
-      <c r="AC41" s="3">
-        <f>COUNTIFS($C$21:$C$500,$J41,$E$21:$E$500,$K41,$H$21:$H$500,"*" &amp; AC$20 &amp; "*")</f>
-        <v>0</v>
-      </c>
-      <c r="AD41" s="3">
-        <f>COUNTIFS($C$21:$C$500,$J41,$E$21:$E$500,$K41,$H$21:$H$500,"*" &amp; AD$20 &amp; "*")</f>
-        <v>0</v>
-      </c>
-      <c r="AE41" s="3">
-        <f>COUNTIFS($C$21:$C$500,$J41,$E$21:$E$500,$K41,$H$21:$H$500,"*" &amp; AE$20 &amp; "*")</f>
-        <v>0</v>
-      </c>
-      <c r="AF41" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AG41" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AH41" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AI41" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AJ41" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AK41" s="28">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AL41" s="45">
-        <f>SUM(L41:AE41)</f>
+      <c r="AL41" s="42">
+        <f t="shared" ref="AL41:AL46" si="8">SUM(L41:AK41)</f>
         <v>0</v>
       </c>
     </row>
@@ -4074,115 +4046,115 @@
       <c r="J42" s="9">
         <v>8</v>
       </c>
-      <c r="K42" s="41">
+      <c r="K42" s="38">
         <v>17</v>
       </c>
-      <c r="L42" s="50">
-        <f t="shared" si="2"/>
+      <c r="L42" s="46">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M42" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N42" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="O42" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="P42" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="Q42" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R42" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="S42" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="T42" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="U42" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="V42" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="W42" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="X42" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="Y42" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="Z42" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AA42" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AB42" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AC42" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AD42" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AE42" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AF42" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="U42" s="3">
+      <c r="AG42" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="V42" s="3">
+      <c r="AH42" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="W42" s="3">
+      <c r="AI42" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="X42" s="3">
+      <c r="AJ42" s="3">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="Y42" s="3">
+      <c r="AK42" s="25">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="Z42" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AA42" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AB42" s="3">
-        <f>COUNTIFS($C$21:$C$500,$J42,$E$21:$E$500,$K42,$H$21:$H$500,"*" &amp; AB$20 &amp; "*")</f>
-        <v>0</v>
-      </c>
-      <c r="AC42" s="3">
-        <f>COUNTIFS($C$21:$C$500,$J42,$E$21:$E$500,$K42,$H$21:$H$500,"*" &amp; AC$20 &amp; "*")</f>
-        <v>0</v>
-      </c>
-      <c r="AD42" s="3">
-        <f>COUNTIFS($C$21:$C$500,$J42,$E$21:$E$500,$K42,$H$21:$H$500,"*" &amp; AD$20 &amp; "*")</f>
-        <v>0</v>
-      </c>
-      <c r="AE42" s="3">
-        <f>COUNTIFS($C$21:$C$500,$J42,$E$21:$E$500,$K42,$H$21:$H$500,"*" &amp; AE$20 &amp; "*")</f>
-        <v>0</v>
-      </c>
-      <c r="AF42" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AG42" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AH42" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AI42" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AJ42" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AK42" s="28">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AL42" s="45">
-        <f>SUM(L42:AE42)</f>
+      <c r="AL42" s="42">
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -4198,115 +4170,115 @@
       <c r="J43" s="9">
         <v>8</v>
       </c>
-      <c r="K43" s="41">
+      <c r="K43" s="38">
         <v>18</v>
       </c>
-      <c r="L43" s="50">
-        <f t="shared" si="2"/>
+      <c r="L43" s="46">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M43" s="3">
-        <f t="shared" ref="M42:AA47" si="5">COUNTIFS($C$21:$C$500,$J43,$E$21:$E$500,$K43,$H$21:$H$500,M$20)</f>
+        <f t="shared" ref="M43:AA47" si="9">COUNTIFS($C$21:$C$500,$J43,$E$21:$E$500,$K43,$H$21:$H$500,M$20)</f>
         <v>0</v>
       </c>
       <c r="N43" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="O43" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="P43" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="Q43" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="R43" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="S43" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="T43" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="U43" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="V43" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="W43" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="X43" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="Y43" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="Z43" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AA43" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AB43" s="3">
-        <f>COUNTIFS($C$21:$C$500,$J43,$E$21:$E$500,$K43,$H$21:$H$500,"*" &amp; AB$20 &amp; "*")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AC43" s="3">
-        <f>COUNTIFS($C$21:$C$500,$J43,$E$21:$E$500,$K43,$H$21:$H$500,"*" &amp; AC$20 &amp; "*")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AD43" s="3">
-        <f>COUNTIFS($C$21:$C$500,$J43,$E$21:$E$500,$K43,$H$21:$H$500,"*" &amp; AD$20 &amp; "*")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AE43" s="3">
-        <f>COUNTIFS($C$21:$C$500,$J43,$E$21:$E$500,$K43,$H$21:$H$500,"*" &amp; AE$20 &amp; "*")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AF43" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AG43" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AH43" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AI43" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AJ43" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AK43" s="28">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AL43" s="45">
-        <f>SUM(L43:AE43)</f>
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AK43" s="25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AL43" s="42">
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -4322,115 +4294,115 @@
       <c r="J44" s="9">
         <v>8</v>
       </c>
-      <c r="K44" s="41">
+      <c r="K44" s="38">
         <v>19</v>
       </c>
-      <c r="L44" s="50">
-        <f t="shared" si="2"/>
+      <c r="L44" s="46">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M44" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="N44" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="O44" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="P44" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="Q44" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="R44" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="S44" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="T44" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="U44" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="V44" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="W44" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="X44" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="Y44" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="Z44" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AA44" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AB44" s="3">
-        <f>COUNTIFS($C$21:$C$500,$J44,$E$21:$E$500,$K44,$H$21:$H$500,"*" &amp; AB$20 &amp; "*")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AC44" s="3">
-        <f>COUNTIFS($C$21:$C$500,$J44,$E$21:$E$500,$K44,$H$21:$H$500,"*" &amp; AC$20 &amp; "*")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AD44" s="3">
-        <f>COUNTIFS($C$21:$C$500,$J44,$E$21:$E$500,$K44,$H$21:$H$500,"*" &amp; AD$20 &amp; "*")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AE44" s="3">
-        <f>COUNTIFS($C$21:$C$500,$J44,$E$21:$E$500,$K44,$H$21:$H$500,"*" &amp; AE$20 &amp; "*")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AF44" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AG44" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AH44" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AI44" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AJ44" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AK44" s="28">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AL44" s="45">
-        <f>SUM(L44:AE44)</f>
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AK44" s="25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AL44" s="42">
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -4446,115 +4418,115 @@
       <c r="J45" s="9">
         <v>8</v>
       </c>
-      <c r="K45" s="41">
+      <c r="K45" s="38">
         <v>20</v>
       </c>
-      <c r="L45" s="50">
-        <f t="shared" si="2"/>
+      <c r="L45" s="46">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M45" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="N45" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="O45" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="P45" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="Q45" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="R45" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="S45" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="T45" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="U45" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="V45" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="W45" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="X45" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="Y45" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="Z45" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AA45" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AB45" s="3">
-        <f>COUNTIFS($C$21:$C$500,$J45,$E$21:$E$500,$K45,$H$21:$H$500,"*" &amp; AB$20 &amp; "*")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AC45" s="3">
-        <f>COUNTIFS($C$21:$C$500,$J45,$E$21:$E$500,$K45,$H$21:$H$500,"*" &amp; AC$20 &amp; "*")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AD45" s="3">
-        <f>COUNTIFS($C$21:$C$500,$J45,$E$21:$E$500,$K45,$H$21:$H$500,"*" &amp; AD$20 &amp; "*")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AE45" s="3">
-        <f>COUNTIFS($C$21:$C$500,$J45,$E$21:$E$500,$K45,$H$21:$H$500,"*" &amp; AE$20 &amp; "*")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AF45" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AG45" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AH45" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AI45" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AJ45" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AK45" s="28">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AL45" s="45">
-        <f>SUM(L45:AE45)</f>
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AK45" s="25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AL45" s="42">
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -4570,115 +4542,115 @@
       <c r="J46" s="9">
         <v>8</v>
       </c>
-      <c r="K46" s="41">
+      <c r="K46" s="38">
         <v>21</v>
       </c>
-      <c r="L46" s="50">
-        <f t="shared" si="2"/>
+      <c r="L46" s="46">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M46" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="N46" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="O46" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="P46" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="Q46" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="R46" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="S46" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="T46" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="U46" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="V46" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="W46" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="X46" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="Y46" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="Z46" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AA46" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AB46" s="3">
-        <f>COUNTIFS($C$21:$C$500,$J46,$E$21:$E$500,$K46,$H$21:$H$500,"*" &amp; AB$20 &amp; "*")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AC46" s="3">
-        <f>COUNTIFS($C$21:$C$500,$J46,$E$21:$E$500,$K46,$H$21:$H$500,"*" &amp; AC$20 &amp; "*")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AD46" s="3">
-        <f>COUNTIFS($C$21:$C$500,$J46,$E$21:$E$500,$K46,$H$21:$H$500,"*" &amp; AD$20 &amp; "*")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AE46" s="3">
-        <f>COUNTIFS($C$21:$C$500,$J46,$E$21:$E$500,$K46,$H$21:$H$500,"*" &amp; AE$20 &amp; "*")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AF46" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AG46" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AH46" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AI46" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AJ46" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AK46" s="28">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AL46" s="45">
-        <f>SUM(L46:AE46)</f>
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AK46" s="25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AL46" s="42">
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -4694,115 +4666,115 @@
       <c r="J47" s="10">
         <v>8</v>
       </c>
-      <c r="K47" s="42">
+      <c r="K47" s="39">
         <v>22</v>
       </c>
-      <c r="L47" s="51">
-        <f t="shared" si="2"/>
+      <c r="L47" s="47">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M47" s="20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="N47" s="20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="O47" s="20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="P47" s="20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="Q47" s="20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="R47" s="20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="S47" s="20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="T47" s="20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="U47" s="20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="V47" s="20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="W47" s="20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="X47" s="20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="Y47" s="20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="Z47" s="20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AA47" s="20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AB47" s="20">
-        <f>COUNTIFS($C$21:$C$500,$J47,$E$21:$E$500,$K47,$H$21:$H$500,"*" &amp; AB$20 &amp; "*")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AC47" s="20">
-        <f>COUNTIFS($C$21:$C$500,$J47,$E$21:$E$500,$K47,$H$21:$H$500,"*" &amp; AC$20 &amp; "*")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AD47" s="20">
-        <f>COUNTIFS($C$21:$C$500,$J47,$E$21:$E$500,$K47,$H$21:$H$500,"*" &amp; AD$20 &amp; "*")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AE47" s="20">
-        <f>COUNTIFS($C$21:$C$500,$J47,$E$21:$E$500,$K47,$H$21:$H$500,"*" &amp; AE$20 &amp; "*")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="AF47" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AG47" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AH47" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AI47" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AJ47" s="20">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AK47" s="29">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AL47" s="46">
-        <f>SUM(L47:AE47)</f>
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AK47" s="26">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AL47" s="43">
+        <f>SUM(L47:AK47)</f>
         <v>0</v>
       </c>
     </row>
@@ -4815,72 +4787,72 @@
       <c r="F48" s="3"/>
       <c r="G48" s="3"/>
       <c r="H48" s="3"/>
-      <c r="J48" s="54" t="s">
+      <c r="J48" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="K48" s="55"/>
+      <c r="K48" s="54"/>
       <c r="L48" s="23">
-        <f t="shared" ref="L48" si="6">COUNTIFS($C$21:$C$500,J48,$E$21:$E$500,K48,$H$21:$H$500,L47)</f>
+        <f>SUM(L21:L47)</f>
         <v>0</v>
       </c>
       <c r="M48" s="24">
-        <f t="shared" ref="M48:V48" si="7">SUM(M21:M47)</f>
+        <f>SUM(M21:M47)</f>
         <v>0</v>
       </c>
       <c r="N48" s="24">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="M48:S48" si="10">SUM(N21:N47)</f>
         <v>0</v>
       </c>
       <c r="O48" s="24">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="P48" s="24">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Q48" s="24">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="R48" s="24">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="S48" s="24">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="T48" s="24">
-        <f t="shared" ref="T48:AA48" si="8">SUM(T21:T47)</f>
+        <f t="shared" ref="T48:AA48" si="11">SUM(T21:T47)</f>
         <v>0</v>
       </c>
       <c r="U48" s="24">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="V48" s="24">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="W48" s="24">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="X48" s="24">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="Y48" s="24">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="Z48" s="24">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AA48" s="24">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AB48" s="24">
@@ -4900,31 +4872,31 @@
         <v>0</v>
       </c>
       <c r="AF48" s="24">
-        <f t="shared" ref="AF48:AK48" si="9">SUM(AF21:AF47)</f>
+        <f t="shared" ref="AF48:AK48" si="12">SUM(AF21:AF47)</f>
         <v>0</v>
       </c>
       <c r="AG48" s="24">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AH48" s="24">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AI48" s="24">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AJ48" s="24">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AK48" s="24">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="AL48" s="33">
-        <f>SUM(L48:AE48)</f>
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AL48" s="30">
+        <f>SUM(L48:AK48)</f>
         <v>0</v>
       </c>
     </row>
@@ -14643,16 +14615,18 @@
     <mergeCell ref="A18:H18"/>
     <mergeCell ref="J48:K48"/>
   </mergeCells>
-  <conditionalFormatting sqref="AL21:AL48 L21:AE48 AF48:AK48">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="notContainsText" dxfId="3" priority="3" operator="notContains" text="0">
+  <conditionalFormatting sqref="L21:AE48 AL21:AL48 AF48:AK48">
+    <cfRule type="notContainsText" dxfId="2" priority="3" operator="notContains" text="0">
       <formula>ISERROR(SEARCH("0",L21))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L21:AL48">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AF48:AK48">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>